<commit_message>
Added some of the blue alliance api
</commit_message>
<xml_diff>
--- a/output_data.xlsx
+++ b/output_data.xlsx
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3103" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3104" uniqueCount="363">
   <si>
     <t>Ranks</t>
   </si>
@@ -35661,6 +35661,9 @@
       <c r="N1" t="s">
         <v>347</v>
       </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">

</xml_diff>